<commit_message>
Added sort explanation to Metadata XLS sheet
</commit_message>
<xml_diff>
--- a/metadata/metadata_standard.xlsx
+++ b/metadata/metadata_standard.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="39520" windowHeight="23820" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="MASTER" sheetId="1" r:id="rId1"/>
-    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
+    <sheet name="README" sheetId="3" r:id="rId1"/>
+    <sheet name="MASTER" sheetId="1" r:id="rId2"/>
+    <sheet name="Adding new information" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="266">
   <si>
     <t>See: http://www.ebi.ac.uk/ena/submit/mixs-checklists</t>
   </si>
@@ -805,6 +806,27 @@
   </si>
   <si>
     <t>Should include key traits like antibiotic resistance or xenobiotic degradation phenotypes for plasmids, converting genes for phage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This document outlines the metadata standard for the CRC 1182. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metadata requires a set of key/value/unit information. </t>
+  </si>
+  <si>
+    <t>The full ilst also includes infomration about the source of the meta data (from you or the infrastructures of the CRC) and what sort of data should be assigned to each defined key.</t>
+  </si>
+  <si>
+    <t>Key = A key that declares a metadata entry</t>
+  </si>
+  <si>
+    <t>Value = A value that is assigned to a key</t>
+  </si>
+  <si>
+    <t>Unit = A measurement unit, if applicable</t>
+  </si>
+  <si>
+    <t>For a full list of defined keys , please see the tab "MASTER"</t>
   </si>
 </sst>
 </file>
@@ -1184,9 +1206,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10867,11 +10939,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Added READ_LENGTH key to metadata standard
</commit_message>
<xml_diff>
--- a/metadata/metadata_standard.xlsx
+++ b/metadata/metadata_standard.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="39520" windowHeight="23820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="39520" windowHeight="23820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="268">
   <si>
     <t>See: http://www.ebi.ac.uk/ena/submit/mixs-checklists</t>
   </si>
@@ -827,6 +827,12 @@
   </si>
   <si>
     <t>For a full list of defined keys , please see the tab "MASTER"</t>
+  </si>
+  <si>
+    <t>READ_LENGTH</t>
+  </si>
+  <si>
+    <t>Size of reads (e.g. 2x150bp, 2x100bp, 1x75p, etc..)</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1256,9 +1262,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2474,37 +2482,55 @@
       <c r="Z46" s="15"/>
     </row>
     <row r="47" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
+      <c r="A47" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="15"/>
+      <c r="Z47" s="15"/>
     </row>
     <row r="48" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G48" s="6"/>
@@ -2516,16 +2542,14 @@
         <v>50</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="E49" s="1"/>
       <c r="F49" s="6" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
@@ -2536,13 +2560,13 @@
         <v>50</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>129</v>
@@ -2556,16 +2580,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>129</v>
@@ -2579,13 +2600,16 @@
         <v>50</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>129</v>
@@ -2599,13 +2623,13 @@
         <v>50</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>129</v>
@@ -2619,13 +2643,13 @@
         <v>50</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>129</v>
@@ -2639,13 +2663,13 @@
         <v>50</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>129</v>
@@ -2659,13 +2683,13 @@
         <v>50</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>129</v>
@@ -2679,16 +2703,13 @@
         <v>50</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>129</v>
@@ -2702,13 +2723,16 @@
         <v>50</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>129</v>
@@ -2722,16 +2746,13 @@
         <v>50</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>129</v>
@@ -2745,13 +2766,16 @@
         <v>50</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>129</v>
@@ -2765,13 +2789,13 @@
         <v>50</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>129</v>
@@ -2785,13 +2809,13 @@
         <v>50</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>129</v>
@@ -2805,13 +2829,13 @@
         <v>50</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>129</v>
@@ -2825,13 +2849,13 @@
         <v>50</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>129</v>
@@ -2845,13 +2869,13 @@
         <v>50</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>129</v>
@@ -2865,13 +2889,13 @@
         <v>50</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>129</v>
@@ -2885,16 +2909,13 @@
         <v>50</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>129</v>
@@ -2908,13 +2929,16 @@
         <v>50</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>129</v>
@@ -2928,13 +2952,13 @@
         <v>50</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>129</v>
@@ -2948,16 +2972,13 @@
         <v>50</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="E70" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>129</v>
@@ -2971,16 +2992,16 @@
         <v>50</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>129</v>
@@ -2994,13 +3015,16 @@
         <v>50</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>129</v>
@@ -3014,13 +3038,13 @@
         <v>50</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>129</v>
@@ -3034,13 +3058,13 @@
         <v>50</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>129</v>
@@ -3054,13 +3078,13 @@
         <v>50</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>129</v>
@@ -3074,16 +3098,13 @@
         <v>50</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>129</v>
@@ -3097,13 +3118,16 @@
         <v>50</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D77" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="E77" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>129</v>
@@ -3117,13 +3141,13 @@
         <v>50</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>129</v>
@@ -3137,13 +3161,13 @@
         <v>50</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>129</v>
@@ -3157,13 +3181,13 @@
         <v>50</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>129</v>
@@ -3177,13 +3201,13 @@
         <v>50</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>129</v>
@@ -3197,16 +3221,13 @@
         <v>50</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>129</v>
@@ -3220,7 +3241,7 @@
         <v>50</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>55</v>
@@ -3229,7 +3250,7 @@
         <v>201</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>129</v>
@@ -3243,13 +3264,16 @@
         <v>50</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>129</v>
@@ -3263,13 +3287,13 @@
         <v>50</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>129</v>
@@ -3283,16 +3307,13 @@
         <v>50</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>129</v>
@@ -3306,13 +3327,16 @@
         <v>50</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>129</v>
@@ -3326,15 +3350,17 @@
         <v>50</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F88" s="6"/>
+        <v>212</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
@@ -3344,17 +3370,15 @@
         <v>50</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>129</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
@@ -3364,16 +3388,13 @@
         <v>50</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>129</v>
@@ -3387,13 +3408,16 @@
         <v>50</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>129</v>
@@ -3407,13 +3431,13 @@
         <v>50</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>129</v>
@@ -3427,13 +3451,13 @@
         <v>50</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>129</v>
@@ -3447,13 +3471,13 @@
         <v>50</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>129</v>
@@ -3467,13 +3491,13 @@
         <v>50</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>129</v>
@@ -3487,13 +3511,13 @@
         <v>50</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>129</v>
@@ -3507,16 +3531,13 @@
         <v>50</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>232</v>
+        <v>39</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>129</v>
@@ -3530,7 +3551,7 @@
         <v>50</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>55</v>
@@ -3539,7 +3560,7 @@
         <v>232</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>129</v>
@@ -3553,13 +3574,16 @@
         <v>50</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>129</v>
@@ -3573,13 +3597,13 @@
         <v>50</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>129</v>
@@ -3593,13 +3617,13 @@
         <v>50</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>129</v>
@@ -3613,13 +3637,13 @@
         <v>50</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>129</v>
@@ -3633,13 +3657,13 @@
         <v>50</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>129</v>
@@ -3653,13 +3677,13 @@
         <v>50</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>129</v>
@@ -3673,16 +3697,13 @@
         <v>50</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>129</v>
@@ -3696,16 +3717,16 @@
         <v>50</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>251</v>
+      <c r="D106" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>129</v>
@@ -3719,13 +3740,16 @@
         <v>50</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>129</v>
@@ -3739,13 +3763,13 @@
         <v>50</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>129</v>
@@ -3759,13 +3783,13 @@
         <v>50</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>129</v>
@@ -3774,10 +3798,22 @@
       <c r="H109" s="6"/>
       <c r="I109" s="6"/>
     </row>
-    <row r="110" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="6"/>
+    <row r="110" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B110" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G110" s="6"/>
       <c r="H110" s="6"/>
       <c r="I110" s="6"/>
@@ -10933,6 +10969,14 @@
       <c r="G1004" s="6"/>
       <c r="H1004" s="6"/>
       <c r="I1004" s="6"/>
+    </row>
+    <row r="1005" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1005" s="1"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="6"/>
+      <c r="G1005" s="6"/>
+      <c r="H1005" s="6"/>
+      <c r="I1005" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added keys for main contact and main email of sample owner
</commit_message>
<xml_diff>
--- a/metadata/metadata_standard.xlsx
+++ b/metadata/metadata_standard.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="272">
   <si>
     <t>See: http://www.ebi.ac.uk/ena/submit/mixs-checklists</t>
   </si>
@@ -833,6 +833,18 @@
   </si>
   <si>
     <t>Size of reads (e.g. 2x150bp, 2x100bp, 1x75p, etc..)</t>
+  </si>
+  <si>
+    <t>MAIN_CONTACT_NAME</t>
+  </si>
+  <si>
+    <t>MAIN_CONTACT_EMAIL</t>
+  </si>
+  <si>
+    <t>Name of the user</t>
+  </si>
+  <si>
+    <t>Email of the user</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1414,41 +1426,37 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="E9" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="F9" s="13"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>41</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F10" s="13"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1458,13 +1466,13 @@
         <v>50</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>44</v>
@@ -1478,16 +1486,16 @@
         <v>50</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>44</v>
+        <v>56</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1498,13 +1506,13 @@
         <v>50</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>44</v>
@@ -1518,13 +1526,13 @@
         <v>50</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>44</v>
@@ -1538,13 +1546,13 @@
         <v>50</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>44</v>
@@ -1558,13 +1566,13 @@
         <v>50</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>44</v>
@@ -1578,13 +1586,13 @@
         <v>50</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>44</v>
@@ -1598,15 +1606,15 @@
         <v>50</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G18" s="6"/>
@@ -1618,13 +1626,13 @@
         <v>50</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>44</v>
@@ -1638,13 +1646,13 @@
         <v>50</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>44</v>
@@ -1655,16 +1663,16 @@
     </row>
     <row r="21" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>44</v>
@@ -1675,18 +1683,18 @@
     </row>
     <row r="22" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>44</v>
       </c>
       <c r="G22" s="6"/>
@@ -1698,13 +1706,13 @@
         <v>37</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>44</v>
@@ -1718,13 +1726,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>44</v>
@@ -1738,13 +1746,13 @@
         <v>37</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>44</v>
@@ -1758,13 +1766,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>44</v>
@@ -1778,13 +1786,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>44</v>
@@ -1798,13 +1806,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>44</v>
@@ -1818,13 +1826,13 @@
         <v>37</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>44</v>
@@ -1838,13 +1846,13 @@
         <v>37</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>44</v>
@@ -1858,13 +1866,13 @@
         <v>37</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>44</v>
@@ -1878,13 +1886,13 @@
         <v>37</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>44</v>
@@ -1898,13 +1906,13 @@
         <v>37</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>44</v>
@@ -1914,106 +1922,58 @@
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="15" t="s">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="15" t="s">
+      <c r="E34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
-      <c r="U34" s="15"/>
-      <c r="V34" s="15"/>
-      <c r="W34" s="15"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="15"/>
-      <c r="Z34" s="15"/>
-    </row>
-    <row r="35" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="15"/>
-      <c r="Z35" s="15"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
         <v>107</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>44</v>
@@ -2050,14 +2010,14 @@
         <v>107</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F37" s="15" t="s">
         <v>44</v>
@@ -2094,14 +2054,14 @@
         <v>107</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>44</v>
@@ -2138,14 +2098,14 @@
         <v>107</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>44</v>
@@ -2182,14 +2142,14 @@
         <v>107</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F40" s="15" t="s">
         <v>44</v>
@@ -2226,14 +2186,14 @@
         <v>107</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>44</v>
@@ -2270,14 +2230,14 @@
         <v>107</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>44</v>
@@ -2314,14 +2274,14 @@
         <v>107</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>44</v>
@@ -2358,14 +2318,14 @@
         <v>107</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>44</v>
@@ -2402,13 +2362,15 @@
         <v>107</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
+      <c r="E45" s="15" t="s">
+        <v>120</v>
+      </c>
       <c r="F45" s="15" t="s">
         <v>44</v>
       </c>
@@ -2444,13 +2406,15 @@
         <v>107</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
+      <c r="E46" s="15" t="s">
+        <v>121</v>
+      </c>
       <c r="F46" s="15" t="s">
         <v>44</v>
       </c>
@@ -2486,19 +2450,25 @@
         <v>107</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>266</v>
+        <v>58</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D47" s="15"/>
-      <c r="E47" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
@@ -2518,98 +2488,133 @@
       <c r="Z47" s="15"/>
     </row>
     <row r="48" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="15"/>
+    </row>
+    <row r="49" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="15"/>
+    </row>
+    <row r="50" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E50" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F50" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-    </row>
-    <row r="49" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-    </row>
-    <row r="50" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="E51" s="1"/>
       <c r="F51" s="6" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>129</v>
@@ -2618,18 +2623,18 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>129</v>
@@ -2638,18 +2643,21 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>129</v>
@@ -2658,18 +2666,18 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>129</v>
@@ -2678,18 +2686,18 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>129</v>
@@ -2698,18 +2706,18 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>129</v>
@@ -2718,21 +2726,18 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>129</v>
@@ -2741,18 +2746,18 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>129</v>
@@ -2761,21 +2766,21 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>129</v>
@@ -2784,18 +2789,18 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>129</v>
@@ -2804,18 +2809,21 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>129</v>
@@ -2824,18 +2832,18 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>129</v>
@@ -2844,18 +2852,18 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>129</v>
@@ -2869,13 +2877,13 @@
         <v>50</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>129</v>
@@ -2889,13 +2897,13 @@
         <v>50</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>129</v>
@@ -2909,13 +2917,13 @@
         <v>50</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>129</v>
@@ -2929,16 +2937,13 @@
         <v>50</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="E68" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>129</v>
@@ -2952,13 +2957,13 @@
         <v>50</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>129</v>
@@ -2972,13 +2977,16 @@
         <v>50</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D70" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="E70" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>129</v>
@@ -2992,16 +3000,13 @@
         <v>50</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>174</v>
+        <v>39</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>129</v>
@@ -3015,16 +3020,13 @@
         <v>50</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="E72" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>129</v>
@@ -3038,13 +3040,16 @@
         <v>50</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>129</v>
@@ -3058,13 +3063,16 @@
         <v>50</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>129</v>
@@ -3078,13 +3086,13 @@
         <v>50</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>129</v>
@@ -3098,13 +3106,13 @@
         <v>50</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>129</v>
@@ -3118,16 +3126,13 @@
         <v>50</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>129</v>
@@ -3141,13 +3146,13 @@
         <v>50</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>129</v>
@@ -3161,13 +3166,16 @@
         <v>50</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>129</v>
@@ -3181,13 +3189,13 @@
         <v>50</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>129</v>
@@ -3201,13 +3209,13 @@
         <v>50</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>129</v>
@@ -3221,13 +3229,13 @@
         <v>50</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>129</v>
@@ -3241,16 +3249,13 @@
         <v>50</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>129</v>
@@ -3264,16 +3269,13 @@
         <v>50</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>129</v>
@@ -3287,13 +3289,16 @@
         <v>50</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>129</v>
@@ -3307,13 +3312,16 @@
         <v>50</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>129</v>
@@ -3327,16 +3335,13 @@
         <v>50</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>129</v>
@@ -3350,13 +3355,13 @@
         <v>50</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>129</v>
@@ -3370,15 +3375,20 @@
         <v>50</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F89" s="6"/>
+        <v>210</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
@@ -3388,13 +3398,13 @@
         <v>50</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>129</v>
@@ -3408,20 +3418,15 @@
         <v>50</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>129</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
@@ -3431,13 +3436,13 @@
         <v>50</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>129</v>
@@ -3451,13 +3456,16 @@
         <v>50</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>129</v>
@@ -3471,13 +3479,13 @@
         <v>50</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>129</v>
@@ -3491,13 +3499,13 @@
         <v>50</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>129</v>
@@ -3511,13 +3519,13 @@
         <v>50</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>129</v>
@@ -3531,13 +3539,13 @@
         <v>50</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>129</v>
@@ -3551,16 +3559,13 @@
         <v>50</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>232</v>
+        <v>39</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>129</v>
@@ -3574,16 +3579,13 @@
         <v>50</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>232</v>
+        <v>39</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>129</v>
@@ -3597,13 +3599,16 @@
         <v>50</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>129</v>
@@ -3617,13 +3622,16 @@
         <v>50</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>129</v>
@@ -3637,13 +3645,13 @@
         <v>50</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>129</v>
@@ -3657,13 +3665,13 @@
         <v>50</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>129</v>
@@ -3677,13 +3685,13 @@
         <v>50</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>129</v>
@@ -3697,13 +3705,13 @@
         <v>50</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>129</v>
@@ -3717,16 +3725,13 @@
         <v>50</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>129</v>
@@ -3740,16 +3745,13 @@
         <v>50</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>251</v>
+        <v>39</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>129</v>
@@ -3763,13 +3765,16 @@
         <v>50</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>129</v>
@@ -3783,13 +3788,16 @@
         <v>50</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>129</v>
@@ -3803,13 +3811,13 @@
         <v>50</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F110" s="6" t="s">
         <v>129</v>
@@ -3818,18 +3826,42 @@
       <c r="H110" s="6"/>
       <c r="I110" s="6"/>
     </row>
-    <row r="111" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="6"/>
+    <row r="111" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B111" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G111" s="6"/>
       <c r="H111" s="6"/>
       <c r="I111" s="6"/>
     </row>
-    <row r="112" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="6"/>
+    <row r="112" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B112" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G112" s="6"/>
       <c r="H112" s="6"/>
       <c r="I112" s="6"/>
@@ -10977,6 +11009,22 @@
       <c r="G1005" s="6"/>
       <c r="H1005" s="6"/>
       <c r="I1005" s="6"/>
+    </row>
+    <row r="1006" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1006" s="1"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="6"/>
+      <c r="G1006" s="6"/>
+      <c r="H1006" s="6"/>
+      <c r="I1006" s="6"/>
+    </row>
+    <row r="1007" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1007" s="1"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="6"/>
+      <c r="G1007" s="6"/>
+      <c r="H1007" s="6"/>
+      <c r="I1007" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added LIBRARY_ID as metadata key
</commit_message>
<xml_diff>
--- a/metadata/metadata_standard.xlsx
+++ b/metadata/metadata_standard.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="274">
   <si>
     <t>See: http://www.ebi.ac.uk/ena/submit/mixs-checklists</t>
   </si>
@@ -845,6 +845,12 @@
   </si>
   <si>
     <t>Email of the user</t>
+  </si>
+  <si>
+    <t>LIBRARY_ID</t>
+  </si>
+  <si>
+    <t>Library ID used for sequencing (from NGS LIMS)</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1962,62 +1968,44 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="15" t="s">
+      <c r="A36" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
-      <c r="Z36" s="15"/>
+      <c r="E36" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="37" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>107</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="F37" s="15" t="s">
         <v>44</v>
@@ -2054,14 +2042,14 @@
         <v>107</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>44</v>
@@ -2098,14 +2086,14 @@
         <v>107</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>44</v>
@@ -2142,14 +2130,14 @@
         <v>107</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F40" s="15" t="s">
         <v>44</v>
@@ -2186,14 +2174,14 @@
         <v>107</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>44</v>
@@ -2230,14 +2218,14 @@
         <v>107</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>44</v>
@@ -2274,14 +2262,14 @@
         <v>107</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>44</v>
@@ -2318,14 +2306,14 @@
         <v>107</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>44</v>
@@ -2362,14 +2350,14 @@
         <v>107</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>44</v>
@@ -2406,14 +2394,14 @@
         <v>107</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>44</v>
@@ -2450,13 +2438,15 @@
         <v>107</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
+      <c r="E47" s="15" t="s">
+        <v>121</v>
+      </c>
       <c r="F47" s="15" t="s">
         <v>44</v>
       </c>
@@ -2492,7 +2482,7 @@
         <v>107</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>39</v>
@@ -2534,19 +2524,25 @@
         <v>107</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>266</v>
+        <v>122</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D49" s="15"/>
-      <c r="E49" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
@@ -2566,37 +2562,55 @@
       <c r="Z49" s="15"/>
     </row>
     <row r="50" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="F50" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
+      <c r="A50" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
+      <c r="S50" s="15"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="15"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="X50" s="15"/>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="15"/>
     </row>
     <row r="51" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F51" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G51" s="6"/>
@@ -2608,16 +2622,14 @@
         <v>50</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="6" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -2628,13 +2640,13 @@
         <v>50</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>129</v>
@@ -2648,16 +2660,13 @@
         <v>50</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>129</v>
@@ -2671,13 +2680,16 @@
         <v>50</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>129</v>
@@ -2691,13 +2703,13 @@
         <v>50</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>129</v>
@@ -2711,13 +2723,13 @@
         <v>50</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>129</v>
@@ -2731,13 +2743,13 @@
         <v>50</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>129</v>
@@ -2751,13 +2763,13 @@
         <v>50</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>129</v>
@@ -2771,16 +2783,13 @@
         <v>50</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>129</v>
@@ -2794,13 +2803,16 @@
         <v>50</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>129</v>
@@ -2814,16 +2826,13 @@
         <v>50</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>129</v>
@@ -2837,13 +2846,16 @@
         <v>50</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>129</v>
@@ -2857,13 +2869,13 @@
         <v>50</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>129</v>
@@ -2877,13 +2889,13 @@
         <v>50</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>129</v>
@@ -2897,13 +2909,13 @@
         <v>50</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>129</v>
@@ -2917,13 +2929,13 @@
         <v>50</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>129</v>
@@ -2937,13 +2949,13 @@
         <v>50</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>129</v>
@@ -2957,13 +2969,13 @@
         <v>50</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>129</v>
@@ -2977,16 +2989,13 @@
         <v>50</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>129</v>
@@ -3000,13 +3009,16 @@
         <v>50</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>129</v>
@@ -3020,13 +3032,13 @@
         <v>50</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>129</v>
@@ -3040,16 +3052,13 @@
         <v>50</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="E73" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>129</v>
@@ -3063,16 +3072,16 @@
         <v>50</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>129</v>
@@ -3086,13 +3095,16 @@
         <v>50</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>129</v>
@@ -3106,13 +3118,13 @@
         <v>50</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>129</v>
@@ -3126,13 +3138,13 @@
         <v>50</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>129</v>
@@ -3146,13 +3158,13 @@
         <v>50</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>129</v>
@@ -3166,16 +3178,13 @@
         <v>50</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>129</v>
@@ -3189,13 +3198,16 @@
         <v>50</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D80" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="E80" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>129</v>
@@ -3209,13 +3221,13 @@
         <v>50</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>129</v>
@@ -3229,13 +3241,13 @@
         <v>50</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>129</v>
@@ -3249,13 +3261,13 @@
         <v>50</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>129</v>
@@ -3269,13 +3281,13 @@
         <v>50</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>129</v>
@@ -3289,16 +3301,13 @@
         <v>50</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>129</v>
@@ -3312,7 +3321,7 @@
         <v>50</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>55</v>
@@ -3321,7 +3330,7 @@
         <v>201</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>129</v>
@@ -3335,13 +3344,16 @@
         <v>50</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>129</v>
@@ -3355,13 +3367,13 @@
         <v>50</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>129</v>
@@ -3375,16 +3387,13 @@
         <v>50</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>129</v>
@@ -3398,13 +3407,16 @@
         <v>50</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>129</v>
@@ -3418,15 +3430,17 @@
         <v>50</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F91" s="6"/>
+        <v>212</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
@@ -3436,17 +3450,15 @@
         <v>50</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>129</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="F92" s="6"/>
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
@@ -3456,16 +3468,13 @@
         <v>50</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>129</v>
@@ -3479,13 +3488,16 @@
         <v>50</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>129</v>
@@ -3499,13 +3511,13 @@
         <v>50</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>129</v>
@@ -3519,13 +3531,13 @@
         <v>50</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>129</v>
@@ -3539,13 +3551,13 @@
         <v>50</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>129</v>
@@ -3559,13 +3571,13 @@
         <v>50</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>129</v>
@@ -3579,13 +3591,13 @@
         <v>50</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>129</v>
@@ -3599,16 +3611,13 @@
         <v>50</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>232</v>
+        <v>39</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>129</v>
@@ -3622,7 +3631,7 @@
         <v>50</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>55</v>
@@ -3631,7 +3640,7 @@
         <v>232</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>129</v>
@@ -3645,13 +3654,16 @@
         <v>50</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>129</v>
@@ -3665,13 +3677,13 @@
         <v>50</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>129</v>
@@ -3685,13 +3697,13 @@
         <v>50</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>129</v>
@@ -3705,13 +3717,13 @@
         <v>50</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>129</v>
@@ -3725,13 +3737,13 @@
         <v>50</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>129</v>
@@ -3745,13 +3757,13 @@
         <v>50</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>129</v>
@@ -3765,16 +3777,13 @@
         <v>50</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>129</v>
@@ -3788,16 +3797,16 @@
         <v>50</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>251</v>
+      <c r="D109" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>129</v>
@@ -3811,13 +3820,16 @@
         <v>50</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F110" s="6" t="s">
         <v>129</v>
@@ -3831,13 +3843,13 @@
         <v>50</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F111" s="6" t="s">
         <v>129</v>
@@ -3851,13 +3863,13 @@
         <v>50</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>129</v>
@@ -3866,15 +3878,27 @@
       <c r="H112" s="6"/>
       <c r="I112" s="6"/>
     </row>
-    <row r="113" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="6"/>
+    <row r="113" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G113" s="6"/>
       <c r="H113" s="6"/>
       <c r="I113" s="6"/>
     </row>
-    <row r="114" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="6"/>
@@ -3882,7 +3906,7 @@
       <c r="H114" s="6"/>
       <c r="I114" s="6"/>
     </row>
-    <row r="115" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="6"/>
@@ -3890,7 +3914,7 @@
       <c r="H115" s="6"/>
       <c r="I115" s="6"/>
     </row>
-    <row r="116" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="6"/>
@@ -3898,7 +3922,7 @@
       <c r="H116" s="6"/>
       <c r="I116" s="6"/>
     </row>
-    <row r="117" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="6"/>
@@ -3906,7 +3930,7 @@
       <c r="H117" s="6"/>
       <c r="I117" s="6"/>
     </row>
-    <row r="118" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="6"/>
@@ -3914,7 +3938,7 @@
       <c r="H118" s="6"/>
       <c r="I118" s="6"/>
     </row>
-    <row r="119" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="6"/>
@@ -3922,7 +3946,7 @@
       <c r="H119" s="6"/>
       <c r="I119" s="6"/>
     </row>
-    <row r="120" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="6"/>
@@ -3930,7 +3954,7 @@
       <c r="H120" s="6"/>
       <c r="I120" s="6"/>
     </row>
-    <row r="121" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="6"/>
@@ -3938,7 +3962,7 @@
       <c r="H121" s="6"/>
       <c r="I121" s="6"/>
     </row>
-    <row r="122" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="6"/>
@@ -3946,7 +3970,7 @@
       <c r="H122" s="6"/>
       <c r="I122" s="6"/>
     </row>
-    <row r="123" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="6"/>
@@ -3954,7 +3978,7 @@
       <c r="H123" s="6"/>
       <c r="I123" s="6"/>
     </row>
-    <row r="124" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="6"/>
@@ -3962,7 +3986,7 @@
       <c r="H124" s="6"/>
       <c r="I124" s="6"/>
     </row>
-    <row r="125" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="6"/>
@@ -3970,7 +3994,7 @@
       <c r="H125" s="6"/>
       <c r="I125" s="6"/>
     </row>
-    <row r="126" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="6"/>
@@ -3978,7 +4002,7 @@
       <c r="H126" s="6"/>
       <c r="I126" s="6"/>
     </row>
-    <row r="127" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="6"/>
@@ -3986,7 +4010,7 @@
       <c r="H127" s="6"/>
       <c r="I127" s="6"/>
     </row>
-    <row r="128" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="6"/>
@@ -11025,6 +11049,14 @@
       <c r="G1007" s="6"/>
       <c r="H1007" s="6"/>
       <c r="I1007" s="6"/>
+    </row>
+    <row r="1008" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1008" s="1"/>
+      <c r="E1008" s="1"/>
+      <c r="F1008" s="6"/>
+      <c r="G1008" s="6"/>
+      <c r="H1008" s="6"/>
+      <c r="I1008" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>